<commit_message>
New Green-Kubo ver 3 in C + each particle handled separately
</commit_message>
<xml_diff>
--- a/Viscosity Testing.xlsx
+++ b/Viscosity Testing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>1. N_WATER</t>
   </si>
@@ -116,6 +116,15 @@
   <si>
     <t>V5</t>
   </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
 </sst>
 </file>
 
@@ -180,6 +189,358 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Green-Kubo Zero Shear'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V_avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Green-Kubo Zero Shear'!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5449846949787352E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1308996938995747</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1963495408493621</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26179938779914941</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32724923474893675</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3926990816987242</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45814892864851153</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52359877559829882</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.78539816339744839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Green-Kubo Zero Shear'!$L$2:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0879939999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6228800000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.463695</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.213850000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>109.92639</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-73D8-436D-85B1-7E803C63D954}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="325988808"/>
+        <c:axId val="325989136"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="325988808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="325989136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="325989136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="325988808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -717,7 +1078,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1305,6 +1666,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2337,7 +2738,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2665,10 +3617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2677,7 +3629,7 @@
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2706,13 +3658,19 @@
         <v>28</v>
       </c>
       <c r="L1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2726,8 +3684,37 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2">
+        <v>1.1268</v>
+      </c>
+      <c r="H2">
+        <v>1.1365400000000001</v>
+      </c>
+      <c r="I2">
+        <v>1.1314299999999999</v>
+      </c>
+      <c r="J2">
+        <v>0.98109999999999997</v>
+      </c>
+      <c r="K2">
+        <v>1.0641</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(G2:K2)</f>
+        <v>1.0879939999999999</v>
+      </c>
+      <c r="M2">
+        <f>_xlfn.STDEV.S(G2:K2)</f>
+        <v>6.6608100708547474E-2</v>
+      </c>
+      <c r="N2">
+        <v>42.33</v>
+      </c>
+      <c r="O2">
+        <v>0.31390000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2741,15 +3728,29 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2">
+        <v>6.6228800000000003</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="L3">
+        <f t="shared" ref="L3:L23" si="1">AVERAGE(G3:K3)</f>
+        <v>6.6228800000000003</v>
+      </c>
+      <c r="M3" t="e">
+        <f t="shared" ref="M3:M23" si="2">_xlfn.STDEV.S(G3:K3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N3">
+        <v>47.16</v>
+      </c>
+      <c r="O3">
+        <v>0.34389999999999998</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2768,10 +3769,16 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="L4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M4" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2790,10 +3797,16 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="L5" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2807,8 +3820,22 @@
       <c r="F6">
         <v>4</v>
       </c>
+      <c r="G6">
+        <v>14.8309</v>
+      </c>
+      <c r="H6">
+        <v>14.096489999999999</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>14.463695</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>0.51930629117121263</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2822,8 +3849,16 @@
       <c r="F7">
         <v>5</v>
       </c>
+      <c r="L7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2837,8 +3872,16 @@
       <c r="F8">
         <v>6</v>
       </c>
+      <c r="L8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2852,8 +3895,16 @@
       <c r="F9">
         <v>7</v>
       </c>
+      <c r="L9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2862,13 +3913,24 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0.78539816339744839</v>
+        <v>0.52359877559829882</v>
       </c>
       <c r="F10">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>45.213850000000001</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>45.213850000000001</v>
+      </c>
+      <c r="M10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2876,14 +3938,25 @@
         <v>5</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>0.98174770424681035</v>
+        <f>4/3*PI()*2.5^3*F11/$B$5^3</f>
+        <v>0.78539816339744839</v>
       </c>
       <c r="F11">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>109.92639</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>109.92639</v>
+      </c>
+      <c r="M11" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2891,14 +3964,22 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>1.1780972450961724</v>
+        <f>4/3*PI()*2.5^3*F12/$B$5^3</f>
+        <v>0.98174770424681035</v>
       </c>
       <c r="F12">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="L12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2906,14 +3987,22 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>1.3744467859455345</v>
+        <f>4/3*PI()*2.5^3*F13/$B$5^3</f>
+        <v>1.1780972450961724</v>
       </c>
       <c r="F13">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="L13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2921,14 +4010,22 @@
         <v>110</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>1.5707963267948968</v>
+        <f>4/3*PI()*2.5^3*F14/$B$5^3</f>
+        <v>1.3744467859455345</v>
       </c>
       <c r="F14">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="L14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2936,78 +4033,169 @@
         <v>4.45</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f>4/3*PI()*2.5^3*F15/$B$5^3</f>
+        <v>1.5707963267948968</v>
+      </c>
+      <c r="F15">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>80267</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>80267</v>
+      </c>
+      <c r="M15" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15">
+        <v>285.2</v>
+      </c>
+      <c r="O15">
+        <v>0.89129999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f>4/3*PI()*2.5^3*F16/$B$5^3</f>
         <v>1.7671458676442586</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>27</v>
       </c>
+      <c r="L16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E16">
-        <f t="shared" si="0"/>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f>4/3*PI()*2.5^3*F17/$B$5^3</f>
         <v>1.9634954084936207</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>30</v>
       </c>
+      <c r="L17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17">
-        <f t="shared" si="0"/>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f>4/3*PI()*2.5^3*F18/$B$5^3</f>
         <v>2.028945255443408</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>31</v>
       </c>
+      <c r="L18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18">
-        <f t="shared" si="0"/>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f>4/3*PI()*2.5^3*F19/$B$5^3</f>
         <v>2.0943951023931953</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>32</v>
       </c>
+      <c r="L19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19">
-        <f t="shared" si="0"/>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f>4/3*PI()*2.5^3*F20/$B$5^3</f>
         <v>2.159844949342983</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>33</v>
       </c>
+      <c r="L20" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M20" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E20">
-        <f t="shared" si="0"/>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f>4/3*PI()*2.5^3*F21/$B$5^3</f>
         <v>2.2252947962927703</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>34</v>
       </c>
+      <c r="L21" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M21" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E21">
-        <f t="shared" si="0"/>
+    <row r="22" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f>4/3*PI()*2.5^3*F22/$B$5^3</f>
         <v>2.2907446432425576</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>35</v>
       </c>
+      <c r="L22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E22">
-        <f t="shared" si="0"/>
+    <row r="23" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f>4/3*PI()*2.5^3*F23/$B$5^3</f>
         <v>2.3561944901923448</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <v>36</v>
+      </c>
+      <c r="L23" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3016,7 +4204,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>